<commit_message>
update daata pengeluaran mahad
</commit_message>
<xml_diff>
--- a/Pengeluaran Mahad.xlsx
+++ b/Pengeluaran Mahad.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" activeTab="1"/>
+    <workbookView windowWidth="19890" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117">
   <si>
     <t>No</t>
   </si>
@@ -305,43 +305,67 @@
     <t>B000-4</t>
   </si>
   <si>
+    <t>Uang Sampah April</t>
+  </si>
+  <si>
+    <t>Uang konsumsi rapat</t>
+  </si>
+  <si>
+    <t>Sekretariat</t>
+  </si>
+  <si>
+    <t>Cetak slip gaji</t>
+  </si>
+  <si>
+    <t>Khairul Huda</t>
+  </si>
+  <si>
+    <t>Peralatan kerja bakti</t>
+  </si>
+  <si>
+    <t>Alat semprot santri</t>
+  </si>
+  <si>
+    <t>Ust. Salim</t>
+  </si>
+  <si>
+    <t>Koperasi</t>
+  </si>
+  <si>
+    <t>Modal awal koperasi</t>
+  </si>
+  <si>
+    <t>Mukafaah</t>
+  </si>
+  <si>
+    <t>Abu Umar</t>
+  </si>
+  <si>
+    <t>Mukafaah Abu Umar</t>
+  </si>
+  <si>
+    <t>B000-5</t>
+  </si>
+  <si>
+    <t>Operasional jumat</t>
+  </si>
+  <si>
     <t>Uang Sampah Mei</t>
   </si>
   <si>
-    <t>Uang konsumsi rapat</t>
-  </si>
-  <si>
-    <t>Sekretariat</t>
-  </si>
-  <si>
-    <t>Cetak slip gaji</t>
-  </si>
-  <si>
-    <t>Khairul Huda</t>
-  </si>
-  <si>
-    <t>Peralatan kerja bakti</t>
-  </si>
-  <si>
-    <t>Alat semprot santri</t>
-  </si>
-  <si>
-    <t>Ust. Salim</t>
-  </si>
-  <si>
-    <t>Koperasi</t>
-  </si>
-  <si>
-    <t>Modal awal koperasi</t>
-  </si>
-  <si>
-    <t>Mukafaah</t>
-  </si>
-  <si>
-    <t>Abu Umar</t>
-  </si>
-  <si>
-    <t>Mukafaah Abu Umar</t>
+    <t>Uang parkir jumat</t>
+  </si>
+  <si>
+    <t>Beli HP</t>
+  </si>
+  <si>
+    <t>Mukafaah Abul Ashim</t>
+  </si>
+  <si>
+    <t>Abu Suhailah</t>
+  </si>
+  <si>
+    <t>Pembelian rak koperasi</t>
   </si>
 </sst>
 </file>
@@ -353,8 +377,8 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -376,39 +400,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -420,15 +421,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,15 +438,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,16 +460,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -484,6 +494,44 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -496,31 +544,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,7 +565,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,7 +583,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,73 +733,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,85 +745,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,29 +776,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,23 +816,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -847,151 +851,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1006,7 +1030,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -5423,9 +5447,9 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -6329,7 +6353,7 @@
         <v>95</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D35" s="3">
         <v>42840</v>
@@ -6569,14 +6593,26 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="3">
+        <v>42856</v>
+      </c>
+      <c r="E44" s="4">
+        <v>200000</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2">
@@ -6584,14 +6620,26 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="3">
+        <v>42856</v>
+      </c>
+      <c r="E45" s="4">
+        <v>100000</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2">
@@ -6599,14 +6647,26 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="3">
+        <v>42859</v>
+      </c>
+      <c r="E46" s="4">
+        <v>100000</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2">
@@ -6614,14 +6674,26 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="3">
+        <v>42861</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1616000</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2">
@@ -6629,47 +6701,87 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="3">
+        <v>42861</v>
+      </c>
+      <c r="E48" s="4">
+        <v>285000</v>
+      </c>
       <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+      <c r="G48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="B49" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="3">
+        <v>42861</v>
+      </c>
+      <c r="E49" s="4">
+        <v>565000</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="B50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="3">
+        <v>42861</v>
+      </c>
+      <c r="E50" s="4">
+        <v>700000</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="4"/>
@@ -6682,7 +6794,9 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="4"/>
@@ -6695,7 +6809,9 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
@@ -6708,7 +6824,9 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="4"/>
@@ -6721,7 +6839,9 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="4"/>
@@ -6734,7 +6854,9 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
@@ -6747,7 +6869,9 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
@@ -6760,7 +6884,9 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="4"/>
@@ -6773,7 +6899,9 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
@@ -6786,7 +6914,9 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="4"/>
@@ -6799,7 +6929,9 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="4"/>
@@ -6812,7 +6944,9 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>

</xml_diff>